<commit_message>
buscar en excel funcionando
</commit_message>
<xml_diff>
--- a/filas_coincidentes.xlsx
+++ b/filas_coincidentes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,99 +436,92 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Nombre</t>
+          <t>SAN NICOLAS DISANG S.R.L</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Descripción</t>
+          <t>Unnamed: 1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Reemplazo</t>
+          <t>Unnamed: 2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Precio de venta</t>
+          <t>Unnamed: 3</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Coste</t>
+          <t>Unnamed: 4</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Categoría</t>
+          <t>Unnamed: 5</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 6</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Combustible</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hilux Nueva</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="n">
-        <v>4607.72</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Fram_Lista_General</t>
-        </is>
+          <t>POXILINA</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>10MIN.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>70G</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1431.41</v>
+      </c>
+      <c r="F2" t="n">
+        <v>889.46</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1076.25</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Combustible</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Hilux Nueva (Papel plegado)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
-        <v>4261.12</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Fram_Lista_General</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Combustible</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>VW Passat, Tiguan 2.0 Tdi</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="n">
-        <v>9765.92</v>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Fram_Lista_General</t>
-        </is>
+          <t>POXILINA</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10MIN.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>250G</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>3138.62</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1950.3</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2359.86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>